<commit_message>
update info of RTNF
</commit_message>
<xml_diff>
--- a/P00_Raw/D02_RTNF/Time_interval_between_sessions.xlsx
+++ b/P00_Raw/D02_RTNF/Time_interval_between_sessions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/spring/Documents/Research/Reliability_NPS/P00_Raw/D02_RTNF/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CF295E1-F3BD-754A-B3B8-B20416E50562}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8D35520-06A4-7943-BF58-5D266FF00452}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20860" yWindow="460" windowWidth="12740" windowHeight="18960" xr2:uid="{1D5008A8-EE42-0A4B-AD34-5E6B07146B5C}"/>
   </bookViews>
@@ -523,7 +523,7 @@
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -907,6 +907,9 @@
       <c r="E19" t="s">
         <v>35</v>
       </c>
+      <c r="F19">
+        <v>20</v>
+      </c>
     </row>
     <row r="20" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A20">
@@ -1139,7 +1142,7 @@
       </c>
       <c r="F31">
         <f>AVERAGE(F2:F30)</f>
-        <v>30.25</v>
+        <v>29.896551724137932</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
@@ -1153,7 +1156,7 @@
       </c>
       <c r="F32">
         <f>STDEV(F2:F30)</f>
-        <v>9.7510683175400494</v>
+        <v>9.7627017176387287</v>
       </c>
     </row>
   </sheetData>

</xml_diff>